<commit_message>
Fixed collision speed and testing some stuff
</commit_message>
<xml_diff>
--- a/highscores.xlsx
+++ b/highscores.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -44,10 +44,10 @@
     <t>Steven</t>
   </si>
   <si>
-    <t>Tori :)</t>
-  </si>
-  <si>
     <t>TORI IS MATLAB KING</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -433,55 +433,55 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4">
-        <v>260</v>
+        <v>280</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B5">
-        <v>200</v>
+        <v>260</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>170</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B7">
-        <v>160</v>
+        <v>170</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B8">
-        <v>110</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9">
-        <v>80</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B10">
         <v>80</v>

</xml_diff>

<commit_message>
Added mainMenu, countDown, closeMenu and more
added mainMenu, countDown, closeMenu, added a built in pause method which is currently unused, updated the displays on all these, and basically everything is in the game except sound effects
</commit_message>
<xml_diff>
--- a/highscores.xlsx
+++ b/highscores.xlsx
@@ -47,7 +47,7 @@
     <t>TORI IS MATLAB KING</t>
   </si>
   <si>
-    <t>NA</t>
+    <t>Blaze it</t>
   </si>
 </sst>
 </file>
@@ -425,50 +425,50 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B3">
-        <v>300</v>
+        <v>490</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B4">
-        <v>280</v>
+        <v>420</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B5">
-        <v>260</v>
+        <v>300</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6">
-        <v>200</v>
+        <v>280</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B7">
-        <v>170</v>
+        <v>260</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B8">
-        <v>160</v>
+        <v>200</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -476,15 +476,15 @@
         <v>5</v>
       </c>
       <c r="B9">
-        <v>110</v>
+        <v>180</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B10">
-        <v>80</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Comments and Added replayability to Tron
Added proper credits
Added the play again prompt.
Added comments
</commit_message>
<xml_diff>
--- a/highscores.xlsx
+++ b/highscores.xlsx
@@ -35,9 +35,6 @@
     <t>Steven N</t>
   </si>
   <si>
-    <t>Yo Dawg Crilla</t>
-  </si>
-  <si>
     <t>Shaleen</t>
   </si>
   <si>
@@ -48,6 +45,9 @@
   </si>
   <si>
     <t>Blaze it</t>
+  </si>
+  <si>
+    <t>Yeet</t>
   </si>
 </sst>
 </file>
@@ -425,7 +425,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>490</v>
@@ -433,7 +433,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>420</v>
@@ -449,7 +449,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>280</v>
@@ -457,7 +457,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>260</v>
@@ -465,7 +465,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8">
         <v>200</v>
@@ -473,7 +473,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9">
         <v>180</v>
@@ -481,7 +481,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B10">
         <v>170</v>

</xml_diff>